<commit_message>
added a few more settings
</commit_message>
<xml_diff>
--- a/test/etc/foo.xlsx
+++ b/test/etc/foo.xlsx
@@ -16,17 +16,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Test.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Brady</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,13 +83,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -68,6 +116,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C4"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Age"/>
+    <tableColumn id="3" name="Location"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,21 +417,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>